<commit_message>
code for added new changes
</commit_message>
<xml_diff>
--- a/templates/Examination.xlsx
+++ b/templates/Examination.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Examination" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +50,7 @@
     <t>Marks</t>
   </si>
   <si>
-    <t xml:space="preserve">Question Tye </t>
+    <t>Question Type (MCQ,WRITTEN,MATCH_PAIR)</t>
   </si>
 </sst>
 </file>
@@ -119,8 +122,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -398,13 +429,13 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="43.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>